<commit_message>
fix: creating ministers table
</commit_message>
<xml_diff>
--- a/economic_game_with_passwords.xlsx
+++ b/economic_game_with_passwords.xlsx
@@ -505,7 +505,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>tlYGS</t>
+          <t>K3mjs</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -542,7 +542,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Gy3l8</t>
+          <t>kiz1I</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -575,7 +575,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1CSBk</t>
+          <t>NTOGu</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>A6bYI</t>
+          <t>DJIUF</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -653,7 +653,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>C5v-X</t>
+          <t>I0oVm</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -690,7 +690,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>E6c4N</t>
+          <t>K1rfs</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -727,7 +727,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>lgAsC</t>
+          <t>HJZxQ</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -760,7 +760,7 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Z0s2A</t>
+          <t>kEzuT</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -797,7 +797,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>raELW</t>
+          <t>Alz89</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -834,7 +834,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1_cmW</t>
+          <t>OjxK9</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -875,7 +875,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>ioFcG</t>
+          <t>tL0WP</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -916,7 +916,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>KvTMW</t>
+          <t>_li9K</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -957,7 +957,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>PhO7P</t>
+          <t>aNCVm</t>
         </is>
       </c>
       <c r="I14" t="n">

</xml_diff>